<commit_message>
12 01 2024 code commit
</commit_message>
<xml_diff>
--- a/AzentioAutomationFramework_AnandhULS/TestData/ulsTestData.xlsx
+++ b/AzentioAutomationFramework_AnandhULS/TestData/ulsTestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="75" windowWidth="28755" windowHeight="12600"/>
+    <workbookView xWindow="0" yWindow="75" windowWidth="28755" windowHeight="12600" firstSheet="41" activeTab="41"/>
   </bookViews>
   <sheets>
     <sheet name="ijara_LoginCredentials" sheetId="1" r:id="rId1"/>
@@ -46,20 +46,22 @@
     <sheet name="TW_offering_ExeTrack" sheetId="42" r:id="rId37"/>
     <sheet name="Murabaha_BeneficiaryTestData" sheetId="43" r:id="rId38"/>
     <sheet name="Muraba_beneficiaryExeSheet" sheetId="44" r:id="rId39"/>
-    <sheet name="Ijarah_ExecutionTracker" sheetId="26" r:id="rId40"/>
-    <sheet name="Murabaha_ExecutionTracker" sheetId="27" r:id="rId41"/>
-    <sheet name="Tawruqq_ExecutionTracker" sheetId="28" r:id="rId42"/>
-    <sheet name="NewAppExecution" sheetId="41" r:id="rId43"/>
-    <sheet name="RunnerTest" sheetId="45" r:id="rId44"/>
-    <sheet name="MurabahaPurchaseOrder_TestData" sheetId="46" r:id="rId45"/>
-    <sheet name="ULSExecution" sheetId="47" r:id="rId46"/>
+    <sheet name="Ijarah_FacilityInfo_DE_TestData" sheetId="48" r:id="rId40"/>
+    <sheet name="Ijarah_ExecutionTracker" sheetId="26" r:id="rId41"/>
+    <sheet name="Murabaha_AddressDetails_DE_TD" sheetId="49" r:id="rId42"/>
+    <sheet name="Murabaha_ExecutionTracker" sheetId="27" r:id="rId43"/>
+    <sheet name="Tawruqq_ExecutionTracker" sheetId="28" r:id="rId44"/>
+    <sheet name="NewAppExecution" sheetId="41" r:id="rId45"/>
+    <sheet name="RunnerTest" sheetId="45" r:id="rId46"/>
+    <sheet name="MurabahaPurchaseOrder_TestData" sheetId="46" r:id="rId47"/>
+    <sheet name="ULSExecution" sheetId="47" r:id="rId48"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3306" uniqueCount="669">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3345" uniqueCount="687">
   <si>
     <t>UserName</t>
   </si>
@@ -2066,6 +2068,60 @@
   </si>
   <si>
     <t>userType08</t>
+  </si>
+  <si>
+    <t>Ijarah App Data entry</t>
+  </si>
+  <si>
+    <t>2060</t>
+  </si>
+  <si>
+    <t>userType09</t>
+  </si>
+  <si>
+    <t>AT_FAC_DET_08</t>
+  </si>
+  <si>
+    <t>DS01_AT_FAC_DET_08</t>
+  </si>
+  <si>
+    <t>IJALS</t>
+  </si>
+  <si>
+    <t>IJASL</t>
+  </si>
+  <si>
+    <t>AT_FAC_DET_09</t>
+  </si>
+  <si>
+    <t>DS01_AT_FAC_DET_09</t>
+  </si>
+  <si>
+    <t>Dealer 1</t>
+  </si>
+  <si>
+    <t>asset_dealer</t>
+  </si>
+  <si>
+    <t>azentio098@gmail.com</t>
+  </si>
+  <si>
+    <t>AT_MU_ADE_IAD_04</t>
+  </si>
+  <si>
+    <t>DS01_AT_MU_ADE_IAD_04</t>
+  </si>
+  <si>
+    <t>userType10</t>
+  </si>
+  <si>
+    <t>3032</t>
+  </si>
+  <si>
+    <t>Murabah data entry</t>
+  </si>
+  <si>
+    <t>9654427845</t>
   </si>
 </sst>
 </file>
@@ -2206,7 +2262,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -2305,6 +2361,19 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -2314,7 +2383,7 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -2377,6 +2446,14 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Excel_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_" xfId="2"/>
@@ -2673,10 +2750,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O18" sqref="O18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P14" sqref="P14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2684,10 +2761,11 @@
     <col min="1" max="1" width="19.28515625" style="3" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="16.42578125" style="3" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="15.140625" style="3" customWidth="1" collapsed="1"/>
-    <col min="4" max="16384" width="9.140625" style="3" collapsed="1"/>
+    <col min="4" max="4" width="25.85546875" style="3" customWidth="1" collapsed="1"/>
+    <col min="5" max="16384" width="9.140625" style="3" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -2698,7 +2776,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -2709,7 +2787,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -2720,7 +2798,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
         <v>548</v>
       </c>
@@ -2731,7 +2809,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:4">
       <c r="A5" s="1" t="s">
         <v>565</v>
       </c>
@@ -2742,7 +2820,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:4">
       <c r="A6" s="1" t="s">
         <v>600</v>
       </c>
@@ -2753,7 +2831,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
         <v>607</v>
       </c>
@@ -2764,7 +2842,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
         <v>633</v>
       </c>
@@ -2775,7 +2853,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:4">
       <c r="A9" s="49" t="s">
         <v>668</v>
       </c>
@@ -2784,6 +2862,45 @@
       </c>
       <c r="C9" s="48" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="49" t="s">
+        <v>668</v>
+      </c>
+      <c r="B10" s="49">
+        <v>3102</v>
+      </c>
+      <c r="C10" s="48" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="50" t="s">
+        <v>671</v>
+      </c>
+      <c r="B11" s="51" t="s">
+        <v>670</v>
+      </c>
+      <c r="C11" s="52" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="49" t="s">
+        <v>683</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>684</v>
+      </c>
+      <c r="C12" s="48" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="53" t="s">
+        <v>685</v>
       </c>
     </row>
   </sheetData>
@@ -2796,6 +2913,9 @@
     <hyperlink ref="C7" r:id="rId6"/>
     <hyperlink ref="C8" r:id="rId7"/>
     <hyperlink ref="C9" r:id="rId8"/>
+    <hyperlink ref="C10" r:id="rId9"/>
+    <hyperlink ref="C11" r:id="rId10"/>
+    <hyperlink ref="C12" r:id="rId11"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -11101,8 +11221,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:R3"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -11274,9 +11394,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -11529,7 +11647,56 @@
 
 <file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H33"/>
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I38" sqref="I38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="20.85546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24.5703125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19.85546875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="25.42578125" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="34" t="s">
+        <v>245</v>
+      </c>
+      <c r="D1" s="34" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="26" t="s">
+        <v>672</v>
+      </c>
+      <c r="B2" s="26" t="s">
+        <v>673</v>
+      </c>
+      <c r="C2" s="32" t="s">
+        <v>674</v>
+      </c>
+      <c r="D2" s="32" t="s">
+        <v>675</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B41" sqref="B41"/>
@@ -11928,9 +12095,31 @@
         <v>127</v>
       </c>
     </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="26" t="s">
+        <v>672</v>
+      </c>
+      <c r="B34" s="26" t="s">
+        <v>673</v>
+      </c>
+      <c r="C34" s="14" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" s="26" t="s">
+        <v>676</v>
+      </c>
+      <c r="B35" s="26" t="s">
+        <v>677</v>
+      </c>
+      <c r="C35" s="14" t="s">
+        <v>127</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C33">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C35">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>
@@ -11938,12 +12127,77 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H50"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="E47" sqref="E47"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="20.85546875" customWidth="1"/>
+    <col min="2" max="2" width="24.85546875" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" customWidth="1"/>
+    <col min="5" max="6" width="30.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>679</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="6" t="s">
+        <v>681</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>682</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>678</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>311</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>680</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>686</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H51"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -12515,9 +12769,20 @@
         <v>127</v>
       </c>
     </row>
+    <row r="51" spans="1:3">
+      <c r="A51" s="15" t="s">
+        <v>681</v>
+      </c>
+      <c r="B51" s="15" t="s">
+        <v>682</v>
+      </c>
+      <c r="C51" s="38" t="s">
+        <v>127</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C50">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C51">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>
@@ -12526,7 +12791,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H38"/>
   <sheetViews>
@@ -12989,7 +13254,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I108"/>
   <sheetViews>
@@ -14547,7 +14812,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I3"/>
   <sheetViews>
@@ -14645,7 +14910,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C3"/>
   <sheetViews>
@@ -14698,7 +14963,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D124"/>
   <sheetViews>

</xml_diff>

<commit_message>
Class file name changes commit and murabaha asset details code commit
</commit_message>
<xml_diff>
--- a/AzentioAutomationFramework_AnandhULS/TestData/ulsTestData.xlsx
+++ b/AzentioAutomationFramework_AnandhULS/TestData/ulsTestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="75" windowWidth="28755" windowHeight="12600" firstSheet="41" activeTab="41"/>
+    <workbookView xWindow="0" yWindow="75" windowWidth="28755" windowHeight="12600"/>
   </bookViews>
   <sheets>
     <sheet name="ijara_LoginCredentials" sheetId="1" r:id="rId1"/>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3345" uniqueCount="687">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3353" uniqueCount="692">
   <si>
     <t>UserName</t>
   </si>
@@ -2122,6 +2122,21 @@
   </si>
   <si>
     <t>9654427845</t>
+  </si>
+  <si>
+    <t>userType11</t>
+  </si>
+  <si>
+    <t>ijarah_data_check</t>
+  </si>
+  <si>
+    <t>userType12</t>
+  </si>
+  <si>
+    <t>0285</t>
+  </si>
+  <si>
+    <t>Murabaha data check</t>
   </si>
 </sst>
 </file>
@@ -2750,10 +2765,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P14" sqref="P14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2903,6 +2918,34 @@
         <v>685</v>
       </c>
     </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="49" t="s">
+        <v>687</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>684</v>
+      </c>
+      <c r="C13" s="48" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="49" t="s">
+        <v>689</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>690</v>
+      </c>
+      <c r="C14" s="48" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>691</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C3" r:id="rId1"/>
@@ -2916,6 +2959,8 @@
     <hyperlink ref="C10" r:id="rId9"/>
     <hyperlink ref="C11" r:id="rId10"/>
     <hyperlink ref="C12" r:id="rId11"/>
+    <hyperlink ref="C13" r:id="rId12"/>
+    <hyperlink ref="C14" r:id="rId13"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -12131,8 +12176,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>